<commit_message>
Hora de tareas modificada
</commit_message>
<xml_diff>
--- a/Tareas.xlsx
+++ b/Tareas.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Familia\Desktop\Clase\Jose\TimeTableManager\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="3525" yWindow="465" windowWidth="28320" windowHeight="15375"/>
+    <workbookView xWindow="3525" yWindow="465" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,14 +22,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Tareas</t>
   </si>
   <si>
-    <t>Horas</t>
-  </si>
-  <si>
     <t>Crear modelo ER</t>
   </si>
   <si>
@@ -62,9 +54,6 @@
     <t>Crear cuenta GitHub</t>
   </si>
   <si>
-    <t>0.0833</t>
-  </si>
-  <si>
     <t>&lt;--5 min</t>
   </si>
   <si>
@@ -74,9 +63,6 @@
     <t>Clara Adolfo</t>
   </si>
   <si>
-    <t>Clara Adolfo Rafael</t>
-  </si>
-  <si>
     <t>Todos</t>
   </si>
   <si>
@@ -84,12 +70,39 @@
   </si>
   <si>
     <t>Jose</t>
+  </si>
+  <si>
+    <t>Buscar la sintaxis de java para los test</t>
+  </si>
+  <si>
+    <t>Clara</t>
+  </si>
+  <si>
+    <t>Hacer test</t>
+  </si>
+  <si>
+    <t>Pensar qué probar</t>
+  </si>
+  <si>
+    <t>Horas reales</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Horas estimadas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clara Adolfo Rafael </t>
+  </si>
+  <si>
+    <t>Modificar la hoja de tareas</t>
+  </si>
+  <si>
+    <t>Autor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -128,11 +141,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -193,7 +207,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -245,7 +259,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -439,7 +453,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -447,16 +461,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -464,113 +480,172 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>14</v>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>15</v>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
+      <c r="C4">
+        <v>0.5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
-        <v>17</v>
+      <c r="D5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
-        <v>17</v>
+      <c r="D6" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="C9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
+      <c r="B11">
+        <v>0.5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>0.5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>0.5</v>
+      </c>
+      <c r="C14">
+        <v>0.5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Añadida hora estimada hacer test
</commit_message>
<xml_diff>
--- a/Tareas.xlsx
+++ b/Tareas.xlsx
@@ -1,28 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26408"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angelnuneztorron/Desktop/TimeTableManager/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3525" yWindow="465" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="3520" yWindow="460" windowWidth="20740" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>Tareas</t>
   </si>
@@ -453,7 +458,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -461,21 +466,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="40.83203125" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -489,7 +494,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -503,7 +508,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -517,7 +522,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -531,7 +536,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -542,7 +547,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -553,7 +558,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -564,7 +569,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -575,7 +580,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -589,7 +594,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -600,7 +605,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
@@ -611,7 +616,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>19</v>
       </c>
@@ -622,7 +627,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
@@ -633,7 +638,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>23</v>
       </c>
@@ -645,6 +650,17 @@
       </c>
       <c r="D14" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test de la clase profesor corregidos
</commit_message>
<xml_diff>
--- a/Tareas.xlsx
+++ b/Tareas.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Portatil-pc\Desktop\Repo\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="3525" yWindow="465" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="38">
   <si>
     <t>Tareas</t>
   </si>
@@ -138,6 +133,9 @@
   </si>
   <si>
     <t>Crear formato del excel</t>
+  </si>
+  <si>
+    <t>Corregir test</t>
   </si>
 </sst>
 </file>
@@ -495,7 +493,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -503,18 +501,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.25" customWidth="1"/>
+    <col min="1" max="1" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.375" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -925,6 +923,23 @@
         <v>42648</v>
       </c>
     </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="5">
+        <v>42652</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
tareas+ test de clase en verde
</commit_message>
<xml_diff>
--- a/Tareas.xlsx
+++ b/Tareas.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
   <si>
     <t>Tareas</t>
   </si>
@@ -149,10 +149,7 @@
     <t>Poner todos los tests en una suite para su ejecución</t>
   </si>
   <si>
-    <t>Crear nuevos tests</t>
-  </si>
-  <si>
-    <t>??</t>
+    <t>Pasar Test pendiente de clase a verde</t>
   </si>
 </sst>
 </file>
@@ -273,7 +270,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -325,7 +322,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -530,7 +527,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,15 +1002,29 @@
         <v>40</v>
       </c>
       <c r="B31">
-        <v>3</v>
-      </c>
-      <c r="C31" t="s">
-        <v>41</v>
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
       </c>
       <c r="D31" t="s">
         <v>27</v>
       </c>
       <c r="E31" s="5">
+        <v>42654</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="D32" t="s">
+        <v>27</v>
+      </c>
+      <c r="E32" s="5">
         <v>42654</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Añadido predicado para comprobar el solape de asignaturas
</commit_message>
<xml_diff>
--- a/Tareas.xlsx
+++ b/Tareas.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Repositorio\TimeTableManager\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="3525" yWindow="465" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
   <si>
     <t>Tareas</t>
   </si>
@@ -150,12 +145,21 @@
   </si>
   <si>
     <t>Pasar Test pendiente de clase a verde</t>
+  </si>
+  <si>
+    <t>Preguntar a Mariano</t>
+  </si>
+  <si>
+    <t>todos</t>
+  </si>
+  <si>
+    <t>Predicado en Prolog para comprobar si se solapan asignaturas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -270,7 +274,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -322,7 +326,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -516,7 +520,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -524,18 +528,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.25" customWidth="1"/>
+    <col min="1" max="1" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.375" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -1028,8 +1032,39 @@
         <v>42654</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D33" s="6"/>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>0.5</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33" s="5">
+        <v>42656</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>0.5</v>
+      </c>
+      <c r="D34" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" s="5">
+        <v>42656</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
numero maximo y min de horas a la semana, no funciona
</commit_message>
<xml_diff>
--- a/Tareas.xlsx
+++ b/Tareas.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="61">
   <si>
     <t>Tareas</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>restriccion max y min numero de horas por semana</t>
+  </si>
+  <si>
+    <t>investigar sobre algoritmos de busqueda con un agente</t>
   </si>
 </sst>
 </file>
@@ -568,7 +571,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -576,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1329,6 +1332,23 @@
         <v>17</v>
       </c>
     </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48" t="s">
+        <v>17</v>
+      </c>
+      <c r="E48" s="5">
+        <v>42670</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
numero max y min de horas funcionando
</commit_message>
<xml_diff>
--- a/Tareas.xlsx
+++ b/Tareas.xlsx
@@ -571,7 +571,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -582,7 +582,7 @@
   <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1328,8 +1328,14 @@
       <c r="B47">
         <v>2</v>
       </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
       <c r="D47" t="s">
         <v>17</v>
+      </c>
+      <c r="E47" s="5">
+        <v>42700</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Maximo numero de horas seguidas de un profesor al dia
</commit_message>
<xml_diff>
--- a/Tareas.xlsx
+++ b/Tareas.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="62">
   <si>
     <t>Tareas</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>investigar sobre algoritmos de busqueda con un agente</t>
+  </si>
+  <si>
+    <t>Maximo numero de horas seguidas de clase profesor</t>
   </si>
 </sst>
 </file>
@@ -571,7 +574,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -579,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1355,6 +1358,20 @@
         <v>42670</v>
       </c>
     </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="D49" t="s">
+        <v>17</v>
+      </c>
+      <c r="E49" s="5">
+        <v>42701</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
maximos gaps al dia
</commit_message>
<xml_diff>
--- a/Tareas.xlsx
+++ b/Tareas.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="63">
   <si>
     <t>Tareas</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>Maximo numero de horas seguidas de clase profesor</t>
+  </si>
+  <si>
+    <t>Max gaps por dia</t>
   </si>
 </sst>
 </file>
@@ -582,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1365,10 +1368,30 @@
       <c r="B49">
         <v>1</v>
       </c>
+      <c r="C49">
+        <v>2</v>
+      </c>
       <c r="D49" t="s">
         <v>17</v>
       </c>
       <c r="E49" s="5">
+        <v>42701</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50" t="s">
+        <v>17</v>
+      </c>
+      <c r="E50" s="5">
         <v>42701</v>
       </c>
     </row>

</xml_diff>

<commit_message>
max y min numero de dias entre sesiones
</commit_message>
<xml_diff>
--- a/Tareas.xlsx
+++ b/Tareas.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="65">
   <si>
     <t>Tareas</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>Max gaps por semana</t>
+  </si>
+  <si>
+    <t>Horas entre sesiones</t>
   </si>
 </sst>
 </file>
@@ -580,7 +583,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -588,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1415,6 +1418,23 @@
         <v>42701</v>
       </c>
     </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52" t="s">
+        <v>17</v>
+      </c>
+      <c r="E52" s="5">
+        <v>42702</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>